<commit_message>
Made the rsi indicator behave according to an Excel spreadsheet prototype.
</commit_message>
<xml_diff>
--- a/src/test/data/STW-rsi-test.xlsx
+++ b/src/test/data/STW-rsi-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\github\data-forge\data-forge-indicators\src\test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C81E8508-94B3-436B-9E7F-0D09CAA2F47D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{78CEB624-A01D-4811-997B-CE204DE5E78C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -40,9 +40,6 @@
     <t>volume</t>
   </si>
   <si>
-    <t>chane</t>
-  </si>
-  <si>
     <t>gain</t>
   </si>
   <si>
@@ -59,6 +56,9 @@
   </si>
   <si>
     <t>rsi</t>
+  </si>
+  <si>
+    <t>change</t>
   </si>
 </sst>
 </file>
@@ -8603,7 +8603,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>chane</c:v>
+                        <c:v>change</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -20647,14 +20647,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M253"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A228" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -20677,25 +20678,25 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>